<commit_message>
feat:se agregaron nuevas funciones con playwrigth tambien forzando los errores con opera
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,31 @@
           <t>validacion medidor</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>cliente</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>marca de medidor extraido</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>modelo medidor extraido</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>medidor extraido opera</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>validacion medidor</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -545,6 +570,19 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>110394374</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -586,6 +624,19 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>556127</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -627,6 +678,19 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>733277</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -668,6 +732,19 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>2493619</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -709,6 +786,19 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>98167619</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -750,6 +840,19 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>644473</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -791,6 +894,27 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>2616329</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -832,6 +956,19 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>277230019</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -873,6 +1010,19 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>2272064</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -914,6 +1064,19 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>2105172</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -955,6 +1118,19 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>744398</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -996,6 +1172,27 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>2494591</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Medidor</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>HEXING</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1037,6 +1234,27 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>2373556</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>JOSE WILLIAN MENDIETA RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2373556</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>CL 72 F NO 111 - 19 PI 2</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1078,6 +1296,27 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>1677822</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>1677822</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>GESTION HABITAT</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>1677822</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1119,6 +1358,19 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>137591</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1161,6 +1413,27 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>2401156</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>2401156</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>CARLOS MOISES ROSAS</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1202,6 +1475,19 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>2796516</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1243,6 +1529,27 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>2552479</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>DORA INES FORERO DE ROJAS</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2552479</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>KR 99 B NO 64 G - 10</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1284,6 +1591,27 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>108666263</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1325,6 +1653,27 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>390818</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Industrial</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1366,6 +1715,27 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>554673</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>KR 68 H NO 67 B - 12</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>554673</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>ORJUELA V.FRANCISCOS</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1407,6 +1777,19 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>761138</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1448,6 +1831,19 @@
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>300058462</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1489,6 +1885,31 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>438485</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>ENEL</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>KR 6 NO 49 - 65 AP 301</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>438485</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1530,6 +1951,19 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>564011</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1572,6 +2006,27 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>364018</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>364018</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>TERRE DES HOMMES DEUTSCHLAND EV</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>364018</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1613,6 +2068,27 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>313841</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>313841</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>CLEMENCIA GAMBA DE CASTILLO</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>313841</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1654,6 +2130,19 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>532728</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1697,6 +2186,27 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>381263</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>KR 51 NO 4 A - 73</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>381263</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>C CURTIDOR</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1738,6 +2248,27 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>2304792</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>CONSTRUCTORA SAN JOSE LTDA</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>2304792</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>KR 21 NO 9 A - 31 LC 43</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1779,6 +2310,27 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>2304783</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>CONSTRUCTORA SAN JOSE LTDA</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>2304783</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>KR 21 NO 9 A - 31 LC 47</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1820,6 +2372,19 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>2304885</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1861,6 +2426,27 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>2304814</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>CONSTRUCTORA SAN JOSE LTDA</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>2304814</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>KR 21 NO 9 A - 31 LC 51</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1902,6 +2488,23 @@
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>2304773</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>2304773</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>KR 21 NO 9 A - 31 LC 144</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1943,6 +2546,27 @@
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>2304904</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>CENTRO COMERCIAL SAN JOSE</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>2304904</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1984,6 +2608,27 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>96926746</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Medidor</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>HEXING</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>HXE12</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2025,6 +2670,27 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>96926790</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>CONSTRUMAX</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>3198177</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>CL 70 A BIS A NO 116 C - 21 BQ 3 AP 201</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2066,6 +2732,27 @@
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>96926878</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>FLORIDA DE ENGATIVA 1</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2107,6 +2794,19 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>96926938</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2148,6 +2848,27 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>106502374</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>CL 66 NO 50 B - 05 AP 301</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2189,6 +2910,19 @@
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>978988</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2230,6 +2964,27 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>2517130</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2271,6 +3026,27 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>1359207</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Medidor</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>HEXING</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>HXE12</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2312,6 +3088,27 @@
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>1359208</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Comercial</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2353,6 +3150,27 @@
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>96926866</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2394,6 +3212,27 @@
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>500526</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>INT 1</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>500526</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2435,6 +3274,19 @@
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>2335072</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2476,6 +3328,19 @@
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>2305017</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2517,6 +3382,27 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>700559</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>MANUEL ANTONIO SANABRIA ROA</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>700559</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>KR 66 NO 107 - 52</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2558,6 +3444,19 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>492684</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2599,6 +3498,19 @@
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>2305029</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2640,6 +3552,19 @@
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>2517073</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2681,6 +3606,27 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>2638108</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Residencial</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>Básica</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>MRSEN1</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2722,6 +3668,19 @@
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>2668365</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2763,6 +3722,23 @@
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
       <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>2668449</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>2668449</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>2668449</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2804,6 +3780,27 @@
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>
       <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>1627963</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>CL 75 NO 80 B - 17 AP 200</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>LUIS A MOJICA A</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>1627963</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2845,6 +3842,19 @@
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>700552</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2886,6 +3896,19 @@
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
       <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>493596</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2927,6 +3950,27 @@
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
       <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>93268239</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>HERMENCIA MARTINEZ</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Medidor</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2968,6 +4012,11 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3009,6 +4058,11 @@
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
       <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>